<commit_message>
Remplacement du dossier par la nouvelle version
</commit_message>
<xml_diff>
--- a/resultats_analyses/metriques/metriques_ptf_arbitre.xlsx
+++ b/resultats_analyses/metriques/metriques_ptf_arbitre.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>13.10%</t>
+          <t>18.67%</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -466,7 +466,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14.03%</t>
+          <t>14.85%</t>
         </is>
       </c>
     </row>

</xml_diff>